<commit_message>
-Changing the MC with STM32G0
</commit_message>
<xml_diff>
--- a/Rlease/BOM/H3BR6 BOM.xlsx
+++ b/Rlease/BOM/H3BR6 BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Hexabitz\H3BR6x-Hardware\Rlease\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules Hardware Design\H3BR6x-Hardware-main\H3BR6x-Hardware-main\Rlease\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C892A9-0E21-46F2-9D66-1967FEC390CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H3BR6_Hardware_ListByValues" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
   <si>
     <t>Qty</t>
   </si>
@@ -42,24 +43,12 @@
     <t>1.00uF</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>4.7uF</t>
   </si>
   <si>
-    <t>C4, C7</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>100R</t>
   </si>
   <si>
@@ -69,15 +58,9 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C3, C5, C6, C8, C9</t>
-  </si>
-  <si>
     <t>270.0R</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>3661BS</t>
   </si>
   <si>
@@ -144,12 +127,6 @@
     <t>KEMET</t>
   </si>
   <si>
-    <t>C0603C103K5RACTU</t>
-  </si>
-  <si>
-    <t>https://octopart.com/c0603c103k5ractu-kemet-133094?r=sp&amp;s=R_iPBxLnSmGqhkU2rIMFpg</t>
-  </si>
-  <si>
     <t>LED 3mm RED Collor</t>
   </si>
   <si>
@@ -168,66 +145,24 @@
     <t>CC0805KKX7R7BB105</t>
   </si>
   <si>
-    <t>https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp&amp;s=YKl1wwtkROau_X5nniH2ig</t>
-  </si>
-  <si>
-    <t>Cap Tant Solid  SMD 2012</t>
-  </si>
-  <si>
     <t>Murata</t>
   </si>
   <si>
-    <t>GRM21BC81E475KA12L</t>
-  </si>
-  <si>
-    <t>https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ</t>
-  </si>
-  <si>
     <t>RC0603JR-070RL</t>
   </si>
   <si>
-    <t>https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp&amp;s=X2NteqRjRNWrnx42Y0aliA</t>
-  </si>
-  <si>
     <t>Thick Film Resistors - SMD 0603</t>
   </si>
   <si>
-    <t>RC0603FR-07270RL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/search?q=RC0603FR-07270RL&amp;start=0</t>
-  </si>
-  <si>
-    <t>R3,R4, R5, R6, R7, R8, R9, R10, R11, R20, R21, R22, R23, R24, R25, R26</t>
-  </si>
-  <si>
     <t xml:space="preserve">TDK </t>
   </si>
   <si>
-    <t>MMZ1608Y300B</t>
-  </si>
-  <si>
-    <t>https://octopart.com/mmz1608y300b-tdk-368280?r=sp&amp;s=cd9_2ZEqQ9q9UNBuQgHAiA</t>
-  </si>
-  <si>
-    <t>Ferrite Beads Multi-Layer 30Ohm 25% 100MHz 1.5A 50mOhm DCR 0603</t>
-  </si>
-  <si>
-    <t>Red 0603 Clear 54 mcd 2 V Surface Mount ChipLED ;</t>
-  </si>
-  <si>
-    <t>https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp&amp;s=_gcP4_q8T1SC6PJQPTQ9yA</t>
-  </si>
-  <si>
     <t>CSTNE8M00G550000R0</t>
   </si>
   <si>
     <t>https://octopart.com/cstne8m00g550000r0-murata-91406934?r=sp</t>
   </si>
   <si>
-    <t>MURATA   Ceramic Resonator 8MHz ±0.5% (Tol) ±0.2% (Stability) 33pF 40Ohm 3-Pin CSMD</t>
-  </si>
-  <si>
     <t>ON Semiconductor</t>
   </si>
   <si>
@@ -264,28 +199,139 @@
     <t>https://octopart.com/rc0603fr-07100rl-yageo-55402879?r=sp</t>
   </si>
   <si>
-    <t>STM32F091CBU6</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
-    <t>MCU 32-bit ARM Cortex M0 RISC 128KB Flash 2.5V/3.3V 48-Pin UFQFPN EP Frame</t>
-  </si>
-  <si>
-    <t>https://octopart.com/stm32f091cbu6-stmicroelectronics-51988677?r=sp</t>
-  </si>
-  <si>
-    <t>RC0603FR-0710KL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/search?q=RC0603FR-0710KL&amp;currency=USD&amp;specs=0</t>
+    <t>PINHD-1X1</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>87227-1</t>
+  </si>
+  <si>
+    <t>https://octopart.com/87227-1-te+connectivity-39512052?r=sp</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>PINHD-1X3</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>Conn Unshrouded Header HDR 3 POS 2.54mm Solder ST Top Entry Thru-Hole Carton</t>
+  </si>
+  <si>
+    <t>5-146281-3</t>
+  </si>
+  <si>
+    <t>https://octopart.com/5-146281-3-te+connectivity+%2F+amp-39745942?r=sp</t>
+  </si>
+  <si>
+    <t>C1, C3, C5, C6</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R1 ,R4, R5, R6, R7, R8, R9, R10, R11, R20, R21, R22, R23, R24, R25, R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C2, C7</t>
+  </si>
+  <si>
+    <t>PCB Header, Unshrouded, Thru 02 Straight Header, .101, AMPMODU Mod II Series</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>YAGEO [VA]</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp</t>
+  </si>
+  <si>
+    <t>CAP TANT 4.7UF 10V 20% 0805</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>10TPU4R7MSI</t>
+  </si>
+  <si>
+    <t>https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0OHM JUMPER 1/10W 0603</t>
+  </si>
+  <si>
+    <t>YAGEO [VR]</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 0603 270ohms 5% Tol	</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ271V</t>
+  </si>
+  <si>
+    <t>https://octopart.com/erj-3geyj271v-panasonic-55560546?r=sp</t>
+  </si>
+  <si>
+    <t>RES 10 K OHM 5% 0603</t>
+  </si>
+  <si>
+    <t>CRCW060310K0JNEB</t>
+  </si>
+  <si>
+    <t>https://octopart.com/crcw060310k0jneb-vishay-46603269</t>
+  </si>
+  <si>
+    <t>Ind chip Bead Multi-Layer 30 ohms 25% 100MHZ Ferrite 1,5A 0603Punched paper T/R</t>
+  </si>
+  <si>
+    <t>MMZ1608Y300BTA00</t>
+  </si>
+  <si>
+    <t>https://octopart.com/mmz1608y300bta00-tdk-7906990?r=sp</t>
+  </si>
+  <si>
+    <t>STM32G0B1CEU6N</t>
+  </si>
+  <si>
+    <t>MCU 32-Bit ARM Cortex-M0+ RISC 512kByte Flash 1.7V to 3.6V 48-Pin UFQFPN Tray</t>
+  </si>
+  <si>
+    <t>https://octopart.com/stm32g0b1ceu6n-stmicroelectronics-116364672?r=sp</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>Red 0603 130آ° Clear 54 mcd 2 V Surface Mount ChipLED ;</t>
+  </si>
+  <si>
+    <t>https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp&amp;s=0nXJNjGsSbWwqfqWlZv0EA</t>
+  </si>
+  <si>
+    <t>8,0000MHZ 33pF SMD MURATA Resonators</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -808,7 +854,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -823,6 +869,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1146,11 +1198,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,7 +1217,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1173,197 +1225,199 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="G8" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>8</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>57</v>
@@ -1372,205 +1426,229 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>16</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>1</v>
-      </c>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
+        <v>73</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
+        <v>1</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>7</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="D14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>1</v>
-      </c>
       <c r="B15" s="5" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>25</v>
+        <v>96</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>1</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>67</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G7" r:id="rId6"/>
-    <hyperlink ref="G9" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="G16" r:id="rId9"/>
-    <hyperlink ref="G17" r:id="rId10"/>
-    <hyperlink ref="G14" r:id="rId11"/>
-    <hyperlink ref="G13" r:id="rId12"/>
-    <hyperlink ref="G8" r:id="rId13"/>
-    <hyperlink ref="G15" r:id="rId14"/>
-    <hyperlink ref="G10" r:id="rId15"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G3" r:id="rId6" xr:uid="{E9E58B30-4569-4264-AD8E-3A967B67B25C}"/>
+    <hyperlink ref="G6" r:id="rId7" xr:uid="{DD186244-4526-4F91-9FD3-871E2931DFD6}"/>
+    <hyperlink ref="G7" r:id="rId8" display="https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId9" xr:uid="{FF115097-5CEA-4687-BF54-AF7C6CE656FA}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{6A353C32-353B-4225-AE9F-EF5EDFC07823}"/>
+    <hyperlink ref="G11" r:id="rId11" xr:uid="{45EF5994-AD94-4CEC-964F-312D151BE4A1}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{566EFAF5-72D4-417B-8F6B-F3092D7BA10A}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{FF7BD87C-E8B4-4AC0-9EB1-A93A6947558F}"/>
+    <hyperlink ref="G17" r:id="rId14" xr:uid="{CA1B9402-0DFB-4D6B-9E33-677A36F9C533}"/>
+    <hyperlink ref="G18" r:id="rId15" xr:uid="{D2F9F401-AB34-47F6-8C23-E45683D5318F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>

</xml_diff>